<commit_message>
Final Release: Integrated Real EasyOCR, New IOCL Dashboard, and Accuracy Metrics
</commit_message>
<xml_diff>
--- a/data/output/ocr.xlsx
+++ b/data/output/ocr.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F165"/>
+  <dimension ref="A1:F242"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3466,7 +3466,7 @@
         <v>0.005</v>
       </c>
       <c r="F126" s="2" t="n">
-        <v>46015.30790904717</v>
+        <v>46015.30790905093</v>
       </c>
     </row>
     <row r="127">
@@ -3490,7 +3490,7 @@
         <v>0.09089999999999999</v>
       </c>
       <c r="F127" s="2" t="n">
-        <v>46015.30790904717</v>
+        <v>46015.30790905093</v>
       </c>
     </row>
     <row r="128">
@@ -3514,7 +3514,7 @@
         <v>0.0791</v>
       </c>
       <c r="F128" s="2" t="n">
-        <v>46015.30790904717</v>
+        <v>46015.30790905093</v>
       </c>
     </row>
     <row r="129">
@@ -3538,7 +3538,7 @@
         <v>0.0516</v>
       </c>
       <c r="F129" s="2" t="n">
-        <v>46015.30790904717</v>
+        <v>46015.30790905093</v>
       </c>
     </row>
     <row r="130">
@@ -3562,7 +3562,7 @@
         <v>0.2427</v>
       </c>
       <c r="F130" s="2" t="n">
-        <v>46015.30790904717</v>
+        <v>46015.30790905093</v>
       </c>
     </row>
     <row r="131">
@@ -3586,7 +3586,7 @@
         <v>0.0134</v>
       </c>
       <c r="F131" s="2" t="n">
-        <v>46015.30790904717</v>
+        <v>46015.30790905093</v>
       </c>
     </row>
     <row r="132">
@@ -3610,7 +3610,7 @@
         <v>0.0218</v>
       </c>
       <c r="F132" s="2" t="n">
-        <v>46015.30790904717</v>
+        <v>46015.30790905093</v>
       </c>
     </row>
     <row r="133">
@@ -3634,7 +3634,7 @@
         <v>0.0368</v>
       </c>
       <c r="F133" s="2" t="n">
-        <v>46015.30790904717</v>
+        <v>46015.30790905093</v>
       </c>
     </row>
     <row r="134">
@@ -3658,7 +3658,7 @@
         <v>0.1063</v>
       </c>
       <c r="F134" s="2" t="n">
-        <v>46015.30790904717</v>
+        <v>46015.30790905093</v>
       </c>
     </row>
     <row r="135">
@@ -3682,7 +3682,7 @@
         <v>0.3488</v>
       </c>
       <c r="F135" s="2" t="n">
-        <v>46015.30790904717</v>
+        <v>46015.30790905093</v>
       </c>
     </row>
     <row r="136">
@@ -3706,7 +3706,7 @@
         <v>0.0403</v>
       </c>
       <c r="F136" s="2" t="n">
-        <v>46015.30790904717</v>
+        <v>46015.30790905093</v>
       </c>
     </row>
     <row r="137">
@@ -3730,7 +3730,7 @@
         <v>0.0663</v>
       </c>
       <c r="F137" s="2" t="n">
-        <v>46015.30790904717</v>
+        <v>46015.30790905093</v>
       </c>
     </row>
     <row r="138">
@@ -3754,7 +3754,7 @@
         <v>0.4265</v>
       </c>
       <c r="F138" s="2" t="n">
-        <v>46015.30790904717</v>
+        <v>46015.30790905093</v>
       </c>
     </row>
     <row r="139">
@@ -3778,7 +3778,7 @@
         <v>0.0735</v>
       </c>
       <c r="F139" s="2" t="n">
-        <v>46015.30790904717</v>
+        <v>46015.30790905093</v>
       </c>
     </row>
     <row r="140">
@@ -3802,7 +3802,7 @@
         <v>0.6008</v>
       </c>
       <c r="F140" s="2" t="n">
-        <v>46015.30790904717</v>
+        <v>46015.30790905093</v>
       </c>
     </row>
     <row r="141">
@@ -3826,7 +3826,7 @@
         <v>0.1647</v>
       </c>
       <c r="F141" s="2" t="n">
-        <v>46015.30790904717</v>
+        <v>46015.30790905093</v>
       </c>
     </row>
     <row r="142">
@@ -3850,7 +3850,7 @@
         <v>0.0548</v>
       </c>
       <c r="F142" s="2" t="n">
-        <v>46015.30790904717</v>
+        <v>46015.30790905093</v>
       </c>
     </row>
     <row r="143">
@@ -3874,7 +3874,7 @@
         <v>0.0347</v>
       </c>
       <c r="F143" s="2" t="n">
-        <v>46015.30790904717</v>
+        <v>46015.30790905093</v>
       </c>
     </row>
     <row r="144">
@@ -3898,7 +3898,7 @@
         <v>0.0214</v>
       </c>
       <c r="F144" s="2" t="n">
-        <v>46015.30790904717</v>
+        <v>46015.30790905093</v>
       </c>
     </row>
     <row r="145">
@@ -3922,7 +3922,7 @@
         <v>0.2716</v>
       </c>
       <c r="F145" s="2" t="n">
-        <v>46015.30790904717</v>
+        <v>46015.30790905093</v>
       </c>
     </row>
     <row r="146">
@@ -3946,7 +3946,7 @@
         <v>0.4607</v>
       </c>
       <c r="F146" s="2" t="n">
-        <v>46015.30790904717</v>
+        <v>46015.30790905093</v>
       </c>
     </row>
     <row r="147">
@@ -3970,7 +3970,7 @@
         <v>0.0582</v>
       </c>
       <c r="F147" s="2" t="n">
-        <v>46015.30790904717</v>
+        <v>46015.30790905093</v>
       </c>
     </row>
     <row r="148">
@@ -3994,7 +3994,7 @@
         <v>0.1452</v>
       </c>
       <c r="F148" s="2" t="n">
-        <v>46015.30790904717</v>
+        <v>46015.30790905093</v>
       </c>
     </row>
     <row r="149">
@@ -4018,7 +4018,7 @@
         <v>0.3746</v>
       </c>
       <c r="F149" s="2" t="n">
-        <v>46015.30790904717</v>
+        <v>46015.30790905093</v>
       </c>
     </row>
     <row r="150">
@@ -4042,7 +4042,7 @@
         <v>0.7846</v>
       </c>
       <c r="F150" s="2" t="n">
-        <v>46015.30790904717</v>
+        <v>46015.30790905093</v>
       </c>
     </row>
     <row r="151">
@@ -4066,7 +4066,7 @@
         <v>0.011</v>
       </c>
       <c r="F151" s="2" t="n">
-        <v>46015.30790904717</v>
+        <v>46015.30790905093</v>
       </c>
     </row>
     <row r="152">
@@ -4090,7 +4090,7 @@
         <v>0.0731</v>
       </c>
       <c r="F152" s="2" t="n">
-        <v>46015.30790904717</v>
+        <v>46015.30790905093</v>
       </c>
     </row>
     <row r="153">
@@ -4114,7 +4114,7 @@
         <v>0.1241</v>
       </c>
       <c r="F153" s="2" t="n">
-        <v>46015.30790904717</v>
+        <v>46015.30790905093</v>
       </c>
     </row>
     <row r="154">
@@ -4138,7 +4138,7 @@
         <v>0.0126</v>
       </c>
       <c r="F154" s="2" t="n">
-        <v>46015.30790904717</v>
+        <v>46015.30790905093</v>
       </c>
     </row>
     <row r="155">
@@ -4162,7 +4162,7 @@
         <v>0.08749999999999999</v>
       </c>
       <c r="F155" s="2" t="n">
-        <v>46015.30790904717</v>
+        <v>46015.30790905093</v>
       </c>
     </row>
     <row r="156">
@@ -4186,7 +4186,7 @@
         <v>0.6702</v>
       </c>
       <c r="F156" s="2" t="n">
-        <v>46015.30790904717</v>
+        <v>46015.30790905093</v>
       </c>
     </row>
     <row r="157">
@@ -4210,7 +4210,7 @@
         <v>0.0107</v>
       </c>
       <c r="F157" s="2" t="n">
-        <v>46015.30790904717</v>
+        <v>46015.30790905093</v>
       </c>
     </row>
     <row r="158">
@@ -4234,7 +4234,7 @@
         <v>0.1008</v>
       </c>
       <c r="F158" s="2" t="n">
-        <v>46015.30790904717</v>
+        <v>46015.30790905093</v>
       </c>
     </row>
     <row r="159">
@@ -4258,7 +4258,7 @@
         <v>0.4274</v>
       </c>
       <c r="F159" s="2" t="n">
-        <v>46015.30790904717</v>
+        <v>46015.30790905093</v>
       </c>
     </row>
     <row r="160">
@@ -4282,7 +4282,7 @@
         <v>0.07489999999999999</v>
       </c>
       <c r="F160" s="2" t="n">
-        <v>46015.30790904717</v>
+        <v>46015.30790905093</v>
       </c>
     </row>
     <row r="161">
@@ -4306,7 +4306,7 @@
         <v>0.1485</v>
       </c>
       <c r="F161" s="2" t="n">
-        <v>46015.30790904717</v>
+        <v>46015.30790905093</v>
       </c>
     </row>
     <row r="162">
@@ -4330,7 +4330,7 @@
         <v>0.1919</v>
       </c>
       <c r="F162" s="2" t="n">
-        <v>46015.30790904717</v>
+        <v>46015.30790905093</v>
       </c>
     </row>
     <row r="163">
@@ -4354,7 +4354,7 @@
         <v>0.1294</v>
       </c>
       <c r="F163" s="2" t="n">
-        <v>46015.30790904717</v>
+        <v>46015.30790905093</v>
       </c>
     </row>
     <row r="164">
@@ -4378,7 +4378,7 @@
         <v>0.1549</v>
       </c>
       <c r="F164" s="2" t="n">
-        <v>46015.30790904717</v>
+        <v>46015.30790905093</v>
       </c>
     </row>
     <row r="165">
@@ -4402,7 +4402,1855 @@
         <v>0.1519</v>
       </c>
       <c r="F165" s="2" t="n">
-        <v>46015.30790904717</v>
+        <v>46015.30790905093</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="inlineStr">
+        <is>
+          <t>sample1.PNG</t>
+        </is>
+      </c>
+      <c r="B166" t="n">
+        <v>1</v>
+      </c>
+      <c r="C166" t="n">
+        <v>1</v>
+      </c>
+      <c r="D166" t="inlineStr">
+        <is>
+          <t>Table name : daily historical stock prices &amp; volumes</t>
+        </is>
+      </c>
+      <c r="E166" t="n">
+        <v>0.7454</v>
+      </c>
+      <c r="F166" s="2" t="n">
+        <v>46017.42774371999</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="inlineStr">
+        <is>
+          <t>sample1.PNG</t>
+        </is>
+      </c>
+      <c r="B167" t="n">
+        <v>1</v>
+      </c>
+      <c r="C167" t="n">
+        <v>2</v>
+      </c>
+      <c r="D167" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="E167" t="n">
+        <v>0.9962</v>
+      </c>
+      <c r="F167" s="2" t="n">
+        <v>46017.42774371999</v>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="inlineStr">
+        <is>
+          <t>sample1.PNG</t>
+        </is>
+      </c>
+      <c r="B168" t="n">
+        <v>1</v>
+      </c>
+      <c r="C168" t="n">
+        <v>3</v>
+      </c>
+      <c r="D168" t="inlineStr">
+        <is>
+          <t>Open</t>
+        </is>
+      </c>
+      <c r="E168" t="n">
+        <v>0.9983</v>
+      </c>
+      <c r="F168" s="2" t="n">
+        <v>46017.42774371999</v>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="inlineStr">
+        <is>
+          <t>sample1.PNG</t>
+        </is>
+      </c>
+      <c r="B169" t="n">
+        <v>1</v>
+      </c>
+      <c r="C169" t="n">
+        <v>4</v>
+      </c>
+      <c r="D169" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="E169" t="n">
+        <v>1</v>
+      </c>
+      <c r="F169" s="2" t="n">
+        <v>46017.42774371999</v>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="inlineStr">
+        <is>
+          <t>sample1.PNG</t>
+        </is>
+      </c>
+      <c r="B170" t="n">
+        <v>1</v>
+      </c>
+      <c r="C170" t="n">
+        <v>5</v>
+      </c>
+      <c r="D170" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="E170" t="n">
+        <v>0.9408</v>
+      </c>
+      <c r="F170" s="2" t="n">
+        <v>46017.42774371999</v>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="inlineStr">
+        <is>
+          <t>sample1.PNG</t>
+        </is>
+      </c>
+      <c r="B171" t="n">
+        <v>1</v>
+      </c>
+      <c r="C171" t="n">
+        <v>6</v>
+      </c>
+      <c r="D171" t="inlineStr">
+        <is>
+          <t>Close / Last</t>
+        </is>
+      </c>
+      <c r="E171" t="n">
+        <v>0.8614000000000001</v>
+      </c>
+      <c r="F171" s="2" t="n">
+        <v>46017.42774371999</v>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="inlineStr">
+        <is>
+          <t>sample1.PNG</t>
+        </is>
+      </c>
+      <c r="B172" t="n">
+        <v>1</v>
+      </c>
+      <c r="C172" t="n">
+        <v>7</v>
+      </c>
+      <c r="D172" t="inlineStr">
+        <is>
+          <t>Volume</t>
+        </is>
+      </c>
+      <c r="E172" t="n">
+        <v>0.9998</v>
+      </c>
+      <c r="F172" s="2" t="n">
+        <v>46017.42774371999</v>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="inlineStr">
+        <is>
+          <t>sample1.PNG</t>
+        </is>
+      </c>
+      <c r="B173" t="n">
+        <v>1</v>
+      </c>
+      <c r="C173" t="n">
+        <v>8</v>
+      </c>
+      <c r="D173" t="inlineStr">
+        <is>
+          <t>01/042017</t>
+        </is>
+      </c>
+      <c r="E173" t="n">
+        <v>0.8895999999999999</v>
+      </c>
+      <c r="F173" s="2" t="n">
+        <v>46017.42774371999</v>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="inlineStr">
+        <is>
+          <t>sample1.PNG</t>
+        </is>
+      </c>
+      <c r="B174" t="n">
+        <v>1</v>
+      </c>
+      <c r="C174" t="n">
+        <v>9</v>
+      </c>
+      <c r="D174" t="inlineStr">
+        <is>
+          <t>62.48</t>
+        </is>
+      </c>
+      <c r="E174" t="n">
+        <v>0.9716</v>
+      </c>
+      <c r="F174" s="2" t="n">
+        <v>46017.42774371999</v>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="inlineStr">
+        <is>
+          <t>sample1.PNG</t>
+        </is>
+      </c>
+      <c r="B175" t="n">
+        <v>1</v>
+      </c>
+      <c r="C175" t="n">
+        <v>10</v>
+      </c>
+      <c r="D175" t="inlineStr">
+        <is>
+          <t>62.75</t>
+        </is>
+      </c>
+      <c r="E175" t="n">
+        <v>0.9989</v>
+      </c>
+      <c r="F175" s="2" t="n">
+        <v>46017.42774371999</v>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="inlineStr">
+        <is>
+          <t>sample1.PNG</t>
+        </is>
+      </c>
+      <c r="B176" t="n">
+        <v>1</v>
+      </c>
+      <c r="C176" t="n">
+        <v>11</v>
+      </c>
+      <c r="D176" t="inlineStr">
+        <is>
+          <t>62.12</t>
+        </is>
+      </c>
+      <c r="E176" t="n">
+        <v>0.9709</v>
+      </c>
+      <c r="F176" s="2" t="n">
+        <v>46017.42774371999</v>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="inlineStr">
+        <is>
+          <t>sample1.PNG</t>
+        </is>
+      </c>
+      <c r="B177" t="n">
+        <v>1</v>
+      </c>
+      <c r="C177" t="n">
+        <v>12</v>
+      </c>
+      <c r="D177" t="inlineStr">
+        <is>
+          <t>62.3</t>
+        </is>
+      </c>
+      <c r="E177" t="n">
+        <v>0.8463000000000001</v>
+      </c>
+      <c r="F177" s="2" t="n">
+        <v>46017.42774371999</v>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="inlineStr">
+        <is>
+          <t>sample1.PNG</t>
+        </is>
+      </c>
+      <c r="B178" t="n">
+        <v>1</v>
+      </c>
+      <c r="C178" t="n">
+        <v>13</v>
+      </c>
+      <c r="D178" t="inlineStr">
+        <is>
+          <t>21,325.140</t>
+        </is>
+      </c>
+      <c r="E178" t="n">
+        <v>0.6407</v>
+      </c>
+      <c r="F178" s="2" t="n">
+        <v>46017.42774371999</v>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="inlineStr">
+        <is>
+          <t>sample1.PNG</t>
+        </is>
+      </c>
+      <c r="B179" t="n">
+        <v>1</v>
+      </c>
+      <c r="C179" t="n">
+        <v>14</v>
+      </c>
+      <c r="D179" t="inlineStr">
+        <is>
+          <t>01/032017</t>
+        </is>
+      </c>
+      <c r="E179" t="n">
+        <v>0.9949</v>
+      </c>
+      <c r="F179" s="2" t="n">
+        <v>46017.42774371999</v>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="inlineStr">
+        <is>
+          <t>sample1.PNG</t>
+        </is>
+      </c>
+      <c r="B180" t="n">
+        <v>1</v>
+      </c>
+      <c r="C180" t="n">
+        <v>15</v>
+      </c>
+      <c r="D180" t="inlineStr">
+        <is>
+          <t>62.79</t>
+        </is>
+      </c>
+      <c r="E180" t="n">
+        <v>0.9391</v>
+      </c>
+      <c r="F180" s="2" t="n">
+        <v>46017.42774371999</v>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="inlineStr">
+        <is>
+          <t>sample1.PNG</t>
+        </is>
+      </c>
+      <c r="B181" t="n">
+        <v>1</v>
+      </c>
+      <c r="C181" t="n">
+        <v>16</v>
+      </c>
+      <c r="D181" t="inlineStr">
+        <is>
+          <t>62.84</t>
+        </is>
+      </c>
+      <c r="E181" t="n">
+        <v>0.7379</v>
+      </c>
+      <c r="F181" s="2" t="n">
+        <v>46017.42774371999</v>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" t="inlineStr">
+        <is>
+          <t>sample1.PNG</t>
+        </is>
+      </c>
+      <c r="B182" t="n">
+        <v>1</v>
+      </c>
+      <c r="C182" t="n">
+        <v>17</v>
+      </c>
+      <c r="D182" t="inlineStr">
+        <is>
+          <t>62.125</t>
+        </is>
+      </c>
+      <c r="E182" t="n">
+        <v>0.9804</v>
+      </c>
+      <c r="F182" s="2" t="n">
+        <v>46017.42774371999</v>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="inlineStr">
+        <is>
+          <t>sample1.PNG</t>
+        </is>
+      </c>
+      <c r="B183" t="n">
+        <v>1</v>
+      </c>
+      <c r="C183" t="n">
+        <v>18</v>
+      </c>
+      <c r="D183" t="inlineStr">
+        <is>
+          <t>62.58</t>
+        </is>
+      </c>
+      <c r="E183" t="n">
+        <v>0.9938</v>
+      </c>
+      <c r="F183" s="2" t="n">
+        <v>46017.42774371999</v>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" t="inlineStr">
+        <is>
+          <t>sample1.PNG</t>
+        </is>
+      </c>
+      <c r="B184" t="n">
+        <v>1</v>
+      </c>
+      <c r="C184" t="n">
+        <v>19</v>
+      </c>
+      <c r="D184" t="inlineStr">
+        <is>
+          <t>20.655.190</t>
+        </is>
+      </c>
+      <c r="E184" t="n">
+        <v>0.8376</v>
+      </c>
+      <c r="F184" s="2" t="n">
+        <v>46017.42774371999</v>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="inlineStr">
+        <is>
+          <t>sample1.PNG</t>
+        </is>
+      </c>
+      <c r="B185" t="n">
+        <v>1</v>
+      </c>
+      <c r="C185" t="n">
+        <v>20</v>
+      </c>
+      <c r="D185" t="inlineStr">
+        <is>
+          <t>12802016</t>
+        </is>
+      </c>
+      <c r="E185" t="n">
+        <v>0.3903</v>
+      </c>
+      <c r="F185" s="2" t="n">
+        <v>46017.42774371999</v>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" t="inlineStr">
+        <is>
+          <t>sample1.PNG</t>
+        </is>
+      </c>
+      <c r="B186" t="n">
+        <v>1</v>
+      </c>
+      <c r="C186" t="n">
+        <v>21</v>
+      </c>
+      <c r="D186" t="inlineStr">
+        <is>
+          <t>62.96</t>
+        </is>
+      </c>
+      <c r="E186" t="n">
+        <v>0.9227</v>
+      </c>
+      <c r="F186" s="2" t="n">
+        <v>46017.42774371999</v>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" t="inlineStr">
+        <is>
+          <t>sample1.PNG</t>
+        </is>
+      </c>
+      <c r="B187" t="n">
+        <v>1</v>
+      </c>
+      <c r="C187" t="n">
+        <v>22</v>
+      </c>
+      <c r="D187" t="inlineStr">
+        <is>
+          <t>62.99</t>
+        </is>
+      </c>
+      <c r="E187" t="n">
+        <v>0.7383</v>
+      </c>
+      <c r="F187" s="2" t="n">
+        <v>46017.42774371999</v>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" t="inlineStr">
+        <is>
+          <t>sample1.PNG</t>
+        </is>
+      </c>
+      <c r="B188" t="n">
+        <v>1</v>
+      </c>
+      <c r="C188" t="n">
+        <v>23</v>
+      </c>
+      <c r="D188" t="inlineStr">
+        <is>
+          <t>62.03</t>
+        </is>
+      </c>
+      <c r="E188" t="n">
+        <v>0.88</v>
+      </c>
+      <c r="F188" s="2" t="n">
+        <v>46017.42774371999</v>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" t="inlineStr">
+        <is>
+          <t>sample1.PNG</t>
+        </is>
+      </c>
+      <c r="B189" t="n">
+        <v>1</v>
+      </c>
+      <c r="C189" t="n">
+        <v>24</v>
+      </c>
+      <c r="D189" t="inlineStr">
+        <is>
+          <t>62.14</t>
+        </is>
+      </c>
+      <c r="E189" t="n">
+        <v>0.9865</v>
+      </c>
+      <c r="F189" s="2" t="n">
+        <v>46017.42774371999</v>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" t="inlineStr">
+        <is>
+          <t>sample1.PNG</t>
+        </is>
+      </c>
+      <c r="B190" t="n">
+        <v>1</v>
+      </c>
+      <c r="C190" t="n">
+        <v>25</v>
+      </c>
+      <c r="D190" t="inlineStr">
+        <is>
+          <t>25,575,.720</t>
+        </is>
+      </c>
+      <c r="E190" t="n">
+        <v>0.4766</v>
+      </c>
+      <c r="F190" s="2" t="n">
+        <v>46017.42774371999</v>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" t="inlineStr">
+        <is>
+          <t>sample1.PNG</t>
+        </is>
+      </c>
+      <c r="B191" t="n">
+        <v>1</v>
+      </c>
+      <c r="C191" t="n">
+        <v>26</v>
+      </c>
+      <c r="D191" t="inlineStr">
+        <is>
+          <t>[2229122016</t>
+        </is>
+      </c>
+      <c r="E191" t="n">
+        <v>0.2677</v>
+      </c>
+      <c r="F191" s="2" t="n">
+        <v>46017.42774371999</v>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" t="inlineStr">
+        <is>
+          <t>sample1.PNG</t>
+        </is>
+      </c>
+      <c r="B192" t="n">
+        <v>1</v>
+      </c>
+      <c r="C192" t="n">
+        <v>27</v>
+      </c>
+      <c r="D192" t="inlineStr">
+        <is>
+          <t>62.86</t>
+        </is>
+      </c>
+      <c r="E192" t="n">
+        <v>0.5837</v>
+      </c>
+      <c r="F192" s="2" t="n">
+        <v>46017.42774371999</v>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" t="inlineStr">
+        <is>
+          <t>sample1.PNG</t>
+        </is>
+      </c>
+      <c r="B193" t="n">
+        <v>1</v>
+      </c>
+      <c r="C193" t="n">
+        <v>28</v>
+      </c>
+      <c r="D193" t="inlineStr">
+        <is>
+          <t>62.73</t>
+        </is>
+      </c>
+      <c r="E193" t="n">
+        <v>0.9092</v>
+      </c>
+      <c r="F193" s="2" t="n">
+        <v>46017.42774371999</v>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" t="inlineStr">
+        <is>
+          <t>sample1.PNG</t>
+        </is>
+      </c>
+      <c r="B194" t="n">
+        <v>1</v>
+      </c>
+      <c r="C194" t="n">
+        <v>29</v>
+      </c>
+      <c r="D194" t="inlineStr">
+        <is>
+          <t>62.9</t>
+        </is>
+      </c>
+      <c r="E194" t="n">
+        <v>0.6122</v>
+      </c>
+      <c r="F194" s="2" t="n">
+        <v>46017.42774371999</v>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" t="inlineStr">
+        <is>
+          <t>sample1.PNG</t>
+        </is>
+      </c>
+      <c r="B195" t="n">
+        <v>1</v>
+      </c>
+      <c r="C195" t="n">
+        <v>30</v>
+      </c>
+      <c r="D195" t="inlineStr">
+        <is>
+          <t>10,248.460</t>
+        </is>
+      </c>
+      <c r="E195" t="n">
+        <v>0.5913</v>
+      </c>
+      <c r="F195" s="2" t="n">
+        <v>46017.42774371999</v>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" t="inlineStr">
+        <is>
+          <t>sample1.PNG</t>
+        </is>
+      </c>
+      <c r="B196" t="n">
+        <v>1</v>
+      </c>
+      <c r="C196" t="n">
+        <v>31</v>
+      </c>
+      <c r="D196" t="inlineStr">
+        <is>
+          <t>12/2812016</t>
+        </is>
+      </c>
+      <c r="E196" t="n">
+        <v>0.4521</v>
+      </c>
+      <c r="F196" s="2" t="n">
+        <v>46017.42774371999</v>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" t="inlineStr">
+        <is>
+          <t>sample1.PNG</t>
+        </is>
+      </c>
+      <c r="B197" t="n">
+        <v>1</v>
+      </c>
+      <c r="C197" t="n">
+        <v>32</v>
+      </c>
+      <c r="D197" t="inlineStr">
+        <is>
+          <t>63.44</t>
+        </is>
+      </c>
+      <c r="E197" t="n">
+        <v>0.3206</v>
+      </c>
+      <c r="F197" s="2" t="n">
+        <v>46017.42774371999</v>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" t="inlineStr">
+        <is>
+          <t>sample1.PNG</t>
+        </is>
+      </c>
+      <c r="B198" t="n">
+        <v>1</v>
+      </c>
+      <c r="C198" t="n">
+        <v>33</v>
+      </c>
+      <c r="D198" t="inlineStr">
+        <is>
+          <t>62.83</t>
+        </is>
+      </c>
+      <c r="E198" t="n">
+        <v>0.5787</v>
+      </c>
+      <c r="F198" s="2" t="n">
+        <v>46017.42774371999</v>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" t="inlineStr">
+        <is>
+          <t>sample1.PNG</t>
+        </is>
+      </c>
+      <c r="B199" t="n">
+        <v>1</v>
+      </c>
+      <c r="C199" t="n">
+        <v>34</v>
+      </c>
+      <c r="D199" t="inlineStr">
+        <is>
+          <t>62.99</t>
+        </is>
+      </c>
+      <c r="E199" t="n">
+        <v>0.6274</v>
+      </c>
+      <c r="F199" s="2" t="n">
+        <v>46017.42774371999</v>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" t="inlineStr">
+        <is>
+          <t>sample1.PNG</t>
+        </is>
+      </c>
+      <c r="B200" t="n">
+        <v>1</v>
+      </c>
+      <c r="C200" t="n">
+        <v>35</v>
+      </c>
+      <c r="D200" t="inlineStr">
+        <is>
+          <t>14.348.340</t>
+        </is>
+      </c>
+      <c r="E200" t="n">
+        <v>0.6152</v>
+      </c>
+      <c r="F200" s="2" t="n">
+        <v>46017.42774371999</v>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" t="inlineStr">
+        <is>
+          <t>sample1.PNG</t>
+        </is>
+      </c>
+      <c r="B201" t="n">
+        <v>1</v>
+      </c>
+      <c r="C201" t="n">
+        <v>36</v>
+      </c>
+      <c r="D201" t="inlineStr">
+        <is>
+          <t>12/27/2016</t>
+        </is>
+      </c>
+      <c r="E201" t="n">
+        <v>0.4713</v>
+      </c>
+      <c r="F201" s="2" t="n">
+        <v>46017.42774371999</v>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" t="inlineStr">
+        <is>
+          <t>sample1.PNG</t>
+        </is>
+      </c>
+      <c r="B202" t="n">
+        <v>1</v>
+      </c>
+      <c r="C202" t="n">
+        <v>37</v>
+      </c>
+      <c r="D202" t="inlineStr">
+        <is>
+          <t>63.21</t>
+        </is>
+      </c>
+      <c r="E202" t="n">
+        <v>0.9663</v>
+      </c>
+      <c r="F202" s="2" t="n">
+        <v>46017.42774371999</v>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" t="inlineStr">
+        <is>
+          <t>sample1.PNG</t>
+        </is>
+      </c>
+      <c r="B203" t="n">
+        <v>1</v>
+      </c>
+      <c r="C203" t="n">
+        <v>38</v>
+      </c>
+      <c r="D203" t="inlineStr">
+        <is>
+          <t>64.07</t>
+        </is>
+      </c>
+      <c r="E203" t="n">
+        <v>0.5362</v>
+      </c>
+      <c r="F203" s="2" t="n">
+        <v>46017.42774371999</v>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" t="inlineStr">
+        <is>
+          <t>sample1.PNG</t>
+        </is>
+      </c>
+      <c r="B204" t="n">
+        <v>1</v>
+      </c>
+      <c r="C204" t="n">
+        <v>39</v>
+      </c>
+      <c r="D204" t="inlineStr">
+        <is>
+          <t>63.21</t>
+        </is>
+      </c>
+      <c r="E204" t="n">
+        <v>0.9296</v>
+      </c>
+      <c r="F204" s="2" t="n">
+        <v>46017.42774371999</v>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" t="inlineStr">
+        <is>
+          <t>sample1.PNG</t>
+        </is>
+      </c>
+      <c r="B205" t="n">
+        <v>1</v>
+      </c>
+      <c r="C205" t="n">
+        <v>40</v>
+      </c>
+      <c r="D205" t="inlineStr">
+        <is>
+          <t>63.28</t>
+        </is>
+      </c>
+      <c r="E205" t="n">
+        <v>0.9986</v>
+      </c>
+      <c r="F205" s="2" t="n">
+        <v>46017.42774371999</v>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" t="inlineStr">
+        <is>
+          <t>sample1.PNG</t>
+        </is>
+      </c>
+      <c r="B206" t="n">
+        <v>1</v>
+      </c>
+      <c r="C206" t="n">
+        <v>41</v>
+      </c>
+      <c r="D206" t="inlineStr">
+        <is>
+          <t>11,743,650</t>
+        </is>
+      </c>
+      <c r="E206" t="n">
+        <v>0.8334</v>
+      </c>
+      <c r="F206" s="2" t="n">
+        <v>46017.42774371999</v>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" t="inlineStr">
+        <is>
+          <t>sample1.PNG</t>
+        </is>
+      </c>
+      <c r="B207" t="n">
+        <v>1</v>
+      </c>
+      <c r="C207" t="n">
+        <v>42</v>
+      </c>
+      <c r="D207" t="inlineStr">
+        <is>
+          <t>12/2302016</t>
+        </is>
+      </c>
+      <c r="E207" t="n">
+        <v>0.5246</v>
+      </c>
+      <c r="F207" s="2" t="n">
+        <v>46017.42774371999</v>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" t="inlineStr">
+        <is>
+          <t>sample1.PNG</t>
+        </is>
+      </c>
+      <c r="B208" t="n">
+        <v>1</v>
+      </c>
+      <c r="C208" t="n">
+        <v>43</v>
+      </c>
+      <c r="D208" t="inlineStr">
+        <is>
+          <t>63.45</t>
+        </is>
+      </c>
+      <c r="E208" t="n">
+        <v>0.9991</v>
+      </c>
+      <c r="F208" s="2" t="n">
+        <v>46017.42774371999</v>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" t="inlineStr">
+        <is>
+          <t>sample1.PNG</t>
+        </is>
+      </c>
+      <c r="B209" t="n">
+        <v>1</v>
+      </c>
+      <c r="C209" t="n">
+        <v>44</v>
+      </c>
+      <c r="D209" t="inlineStr">
+        <is>
+          <t>63.54</t>
+        </is>
+      </c>
+      <c r="E209" t="n">
+        <v>0.9841</v>
+      </c>
+      <c r="F209" s="2" t="n">
+        <v>46017.42774371999</v>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" t="inlineStr">
+        <is>
+          <t>sample1.PNG</t>
+        </is>
+      </c>
+      <c r="B210" t="n">
+        <v>1</v>
+      </c>
+      <c r="C210" t="n">
+        <v>45</v>
+      </c>
+      <c r="D210" t="inlineStr">
+        <is>
+          <t>62.8</t>
+        </is>
+      </c>
+      <c r="E210" t="n">
+        <v>0.9646</v>
+      </c>
+      <c r="F210" s="2" t="n">
+        <v>46017.42774371999</v>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" t="inlineStr">
+        <is>
+          <t>sample1.PNG</t>
+        </is>
+      </c>
+      <c r="B211" t="n">
+        <v>1</v>
+      </c>
+      <c r="C211" t="n">
+        <v>46</v>
+      </c>
+      <c r="D211" t="inlineStr">
+        <is>
+          <t>63.24</t>
+        </is>
+      </c>
+      <c r="E211" t="n">
+        <v>0.9986</v>
+      </c>
+      <c r="F211" s="2" t="n">
+        <v>46017.42774371999</v>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" t="inlineStr">
+        <is>
+          <t>sample1.PNG</t>
+        </is>
+      </c>
+      <c r="B212" t="n">
+        <v>1</v>
+      </c>
+      <c r="C212" t="n">
+        <v>47</v>
+      </c>
+      <c r="D212" t="inlineStr">
+        <is>
+          <t>12.399.540</t>
+        </is>
+      </c>
+      <c r="E212" t="n">
+        <v>0.6412</v>
+      </c>
+      <c r="F212" s="2" t="n">
+        <v>46017.42774371999</v>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" t="inlineStr">
+        <is>
+          <t>sample1.PNG</t>
+        </is>
+      </c>
+      <c r="B213" t="n">
+        <v>1</v>
+      </c>
+      <c r="C213" t="n">
+        <v>48</v>
+      </c>
+      <c r="D213" t="inlineStr">
+        <is>
+          <t>120222016</t>
+        </is>
+      </c>
+      <c r="E213" t="n">
+        <v>0.4854</v>
+      </c>
+      <c r="F213" s="2" t="n">
+        <v>46017.42774371999</v>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" t="inlineStr">
+        <is>
+          <t>sample1.PNG</t>
+        </is>
+      </c>
+      <c r="B214" t="n">
+        <v>1</v>
+      </c>
+      <c r="C214" t="n">
+        <v>49</v>
+      </c>
+      <c r="D214" t="inlineStr">
+        <is>
+          <t>63.84</t>
+        </is>
+      </c>
+      <c r="E214" t="n">
+        <v>0.8835</v>
+      </c>
+      <c r="F214" s="2" t="n">
+        <v>46017.42774371999</v>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" t="inlineStr">
+        <is>
+          <t>sample1.PNG</t>
+        </is>
+      </c>
+      <c r="B215" t="n">
+        <v>1</v>
+      </c>
+      <c r="C215" t="n">
+        <v>50</v>
+      </c>
+      <c r="D215" t="inlineStr">
+        <is>
+          <t>64.</t>
+        </is>
+      </c>
+      <c r="E215" t="n">
+        <v>0.4165</v>
+      </c>
+      <c r="F215" s="2" t="n">
+        <v>46017.42774371999</v>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" t="inlineStr">
+        <is>
+          <t>sample1.PNG</t>
+        </is>
+      </c>
+      <c r="B216" t="n">
+        <v>1</v>
+      </c>
+      <c r="C216" t="n">
+        <v>51</v>
+      </c>
+      <c r="D216" t="inlineStr">
+        <is>
+          <t>63.405</t>
+        </is>
+      </c>
+      <c r="E216" t="n">
+        <v>0.999</v>
+      </c>
+      <c r="F216" s="2" t="n">
+        <v>46017.42774371999</v>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" t="inlineStr">
+        <is>
+          <t>sample1.PNG</t>
+        </is>
+      </c>
+      <c r="B217" t="n">
+        <v>1</v>
+      </c>
+      <c r="C217" t="n">
+        <v>52</v>
+      </c>
+      <c r="D217" t="inlineStr">
+        <is>
+          <t>63.55</t>
+        </is>
+      </c>
+      <c r="E217" t="n">
+        <v>0.9993</v>
+      </c>
+      <c r="F217" s="2" t="n">
+        <v>46017.42774371999</v>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" t="inlineStr">
+        <is>
+          <t>sample1.PNG</t>
+        </is>
+      </c>
+      <c r="B218" t="n">
+        <v>1</v>
+      </c>
+      <c r="C218" t="n">
+        <v>53</v>
+      </c>
+      <c r="D218" t="inlineStr">
+        <is>
+          <t>22.175.2701</t>
+        </is>
+      </c>
+      <c r="E218" t="n">
+        <v>0.2873</v>
+      </c>
+      <c r="F218" s="2" t="n">
+        <v>46017.42774371999</v>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" t="inlineStr">
+        <is>
+          <t>sample1.PNG</t>
+        </is>
+      </c>
+      <c r="B219" t="n">
+        <v>1</v>
+      </c>
+      <c r="C219" t="n">
+        <v>54</v>
+      </c>
+      <c r="D219" t="inlineStr">
+        <is>
+          <t>120212016</t>
+        </is>
+      </c>
+      <c r="E219" t="n">
+        <v>0.2444</v>
+      </c>
+      <c r="F219" s="2" t="n">
+        <v>46017.42774371999</v>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" t="inlineStr">
+        <is>
+          <t>sample1.PNG</t>
+        </is>
+      </c>
+      <c r="B220" t="n">
+        <v>1</v>
+      </c>
+      <c r="C220" t="n">
+        <v>55</v>
+      </c>
+      <c r="D220" t="inlineStr">
+        <is>
+          <t>63.43</t>
+        </is>
+      </c>
+      <c r="E220" t="n">
+        <v>0.9579</v>
+      </c>
+      <c r="F220" s="2" t="n">
+        <v>46017.42774371999</v>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" t="inlineStr">
+        <is>
+          <t>sample1.PNG</t>
+        </is>
+      </c>
+      <c r="B221" t="n">
+        <v>1</v>
+      </c>
+      <c r="C221" t="n">
+        <v>56</v>
+      </c>
+      <c r="D221" t="inlineStr">
+        <is>
+          <t>63.7</t>
+        </is>
+      </c>
+      <c r="E221" t="n">
+        <v>0.9764</v>
+      </c>
+      <c r="F221" s="2" t="n">
+        <v>46017.42774371999</v>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" t="inlineStr">
+        <is>
+          <t>sample1.PNG</t>
+        </is>
+      </c>
+      <c r="B222" t="n">
+        <v>1</v>
+      </c>
+      <c r="C222" t="n">
+        <v>57</v>
+      </c>
+      <c r="D222" t="inlineStr">
+        <is>
+          <t>63.12</t>
+        </is>
+      </c>
+      <c r="E222" t="n">
+        <v>0.9943</v>
+      </c>
+      <c r="F222" s="2" t="n">
+        <v>46017.42774371999</v>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" t="inlineStr">
+        <is>
+          <t>sample1.PNG</t>
+        </is>
+      </c>
+      <c r="B223" t="n">
+        <v>1</v>
+      </c>
+      <c r="C223" t="n">
+        <v>58</v>
+      </c>
+      <c r="D223" t="inlineStr">
+        <is>
+          <t>63.54</t>
+        </is>
+      </c>
+      <c r="E223" t="n">
+        <v>0.9989</v>
+      </c>
+      <c r="F223" s="2" t="n">
+        <v>46017.42774371999</v>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" t="inlineStr">
+        <is>
+          <t>sample1.PNG</t>
+        </is>
+      </c>
+      <c r="B224" t="n">
+        <v>1</v>
+      </c>
+      <c r="C224" t="n">
+        <v>59</v>
+      </c>
+      <c r="D224" t="inlineStr">
+        <is>
+          <t>17.084.370</t>
+        </is>
+      </c>
+      <c r="E224" t="n">
+        <v>0.6364</v>
+      </c>
+      <c r="F224" s="2" t="n">
+        <v>46017.42774371999</v>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" t="inlineStr">
+        <is>
+          <t>sample1.PNG</t>
+        </is>
+      </c>
+      <c r="B225" t="n">
+        <v>1</v>
+      </c>
+      <c r="C225" t="n">
+        <v>60</v>
+      </c>
+      <c r="D225" t="inlineStr">
+        <is>
+          <t>12/202016</t>
+        </is>
+      </c>
+      <c r="E225" t="n">
+        <v>0.5682</v>
+      </c>
+      <c r="F225" s="2" t="n">
+        <v>46017.42774371999</v>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" t="inlineStr">
+        <is>
+          <t>sample1.PNG</t>
+        </is>
+      </c>
+      <c r="B226" t="n">
+        <v>1</v>
+      </c>
+      <c r="C226" t="n">
+        <v>61</v>
+      </c>
+      <c r="D226" t="inlineStr">
+        <is>
+          <t>63.69</t>
+        </is>
+      </c>
+      <c r="E226" t="n">
+        <v>0.9987</v>
+      </c>
+      <c r="F226" s="2" t="n">
+        <v>46017.42774371999</v>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" t="inlineStr">
+        <is>
+          <t>sample1.PNG</t>
+        </is>
+      </c>
+      <c r="B227" t="n">
+        <v>1</v>
+      </c>
+      <c r="C227" t="n">
+        <v>62</v>
+      </c>
+      <c r="D227" t="inlineStr">
+        <is>
+          <t>63.8</t>
+        </is>
+      </c>
+      <c r="E227" t="n">
+        <v>0.8535</v>
+      </c>
+      <c r="F227" s="2" t="n">
+        <v>46017.42774371999</v>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" t="inlineStr">
+        <is>
+          <t>sample1.PNG</t>
+        </is>
+      </c>
+      <c r="B228" t="n">
+        <v>1</v>
+      </c>
+      <c r="C228" t="n">
+        <v>63</v>
+      </c>
+      <c r="D228" t="inlineStr">
+        <is>
+          <t>63.025</t>
+        </is>
+      </c>
+      <c r="E228" t="n">
+        <v>0.993</v>
+      </c>
+      <c r="F228" s="2" t="n">
+        <v>46017.42774371999</v>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229" t="inlineStr">
+        <is>
+          <t>sample1.PNG</t>
+        </is>
+      </c>
+      <c r="B229" t="n">
+        <v>1</v>
+      </c>
+      <c r="C229" t="n">
+        <v>64</v>
+      </c>
+      <c r="D229" t="inlineStr">
+        <is>
+          <t>63.54</t>
+        </is>
+      </c>
+      <c r="E229" t="n">
+        <v>0.968</v>
+      </c>
+      <c r="F229" s="2" t="n">
+        <v>46017.42774371999</v>
+      </c>
+    </row>
+    <row r="230">
+      <c r="A230" t="inlineStr">
+        <is>
+          <t>sample1.PNG</t>
+        </is>
+      </c>
+      <c r="B230" t="n">
+        <v>1</v>
+      </c>
+      <c r="C230" t="n">
+        <v>65</v>
+      </c>
+      <c r="D230" t="inlineStr">
+        <is>
+          <t>26,017,470</t>
+        </is>
+      </c>
+      <c r="E230" t="n">
+        <v>0.3713</v>
+      </c>
+      <c r="F230" s="2" t="n">
+        <v>46017.42774371999</v>
+      </c>
+    </row>
+    <row r="231">
+      <c r="A231" t="inlineStr">
+        <is>
+          <t>sample1.PNG</t>
+        </is>
+      </c>
+      <c r="B231" t="n">
+        <v>1</v>
+      </c>
+      <c r="C231" t="n">
+        <v>66</v>
+      </c>
+      <c r="D231" t="inlineStr">
+        <is>
+          <t>12/1922016</t>
+        </is>
+      </c>
+      <c r="E231" t="n">
+        <v>0.8508</v>
+      </c>
+      <c r="F231" s="2" t="n">
+        <v>46017.42774371999</v>
+      </c>
+    </row>
+    <row r="232">
+      <c r="A232" t="inlineStr">
+        <is>
+          <t>sample1.PNG</t>
+        </is>
+      </c>
+      <c r="B232" t="n">
+        <v>1</v>
+      </c>
+      <c r="C232" t="n">
+        <v>67</v>
+      </c>
+      <c r="D232" t="inlineStr">
+        <is>
+          <t>62.56</t>
+        </is>
+      </c>
+      <c r="E232" t="n">
+        <v>0.9825</v>
+      </c>
+      <c r="F232" s="2" t="n">
+        <v>46017.42774371999</v>
+      </c>
+    </row>
+    <row r="233">
+      <c r="A233" t="inlineStr">
+        <is>
+          <t>sample1.PNG</t>
+        </is>
+      </c>
+      <c r="B233" t="n">
+        <v>1</v>
+      </c>
+      <c r="C233" t="n">
+        <v>68</v>
+      </c>
+      <c r="D233" t="inlineStr">
+        <is>
+          <t>63.77</t>
+        </is>
+      </c>
+      <c r="E233" t="n">
+        <v>0.9641</v>
+      </c>
+      <c r="F233" s="2" t="n">
+        <v>46017.42774371999</v>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" t="inlineStr">
+        <is>
+          <t>sample1.PNG</t>
+        </is>
+      </c>
+      <c r="B234" t="n">
+        <v>1</v>
+      </c>
+      <c r="C234" t="n">
+        <v>69</v>
+      </c>
+      <c r="D234" t="inlineStr">
+        <is>
+          <t>62.42</t>
+        </is>
+      </c>
+      <c r="E234" t="n">
+        <v>0.6025</v>
+      </c>
+      <c r="F234" s="2" t="n">
+        <v>46017.42774371999</v>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" t="inlineStr">
+        <is>
+          <t>sample1.PNG</t>
+        </is>
+      </c>
+      <c r="B235" t="n">
+        <v>1</v>
+      </c>
+      <c r="C235" t="n">
+        <v>70</v>
+      </c>
+      <c r="D235" t="inlineStr">
+        <is>
+          <t>63.62</t>
+        </is>
+      </c>
+      <c r="E235" t="n">
+        <v>0.9969</v>
+      </c>
+      <c r="F235" s="2" t="n">
+        <v>46017.42774371999</v>
+      </c>
+    </row>
+    <row r="236">
+      <c r="A236" t="inlineStr">
+        <is>
+          <t>sample1.PNG</t>
+        </is>
+      </c>
+      <c r="B236" t="n">
+        <v>1</v>
+      </c>
+      <c r="C236" t="n">
+        <v>71</v>
+      </c>
+      <c r="D236" t="inlineStr">
+        <is>
+          <t>34.318.500</t>
+        </is>
+      </c>
+      <c r="E236" t="n">
+        <v>0.6714</v>
+      </c>
+      <c r="F236" s="2" t="n">
+        <v>46017.42774371999</v>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" t="inlineStr">
+        <is>
+          <t>sample1.PNG</t>
+        </is>
+      </c>
+      <c r="B237" t="n">
+        <v>1</v>
+      </c>
+      <c r="C237" t="n">
+        <v>72</v>
+      </c>
+      <c r="D237" t="inlineStr">
+        <is>
+          <t>12/16/2016</t>
+        </is>
+      </c>
+      <c r="E237" t="n">
+        <v>0.6476</v>
+      </c>
+      <c r="F237" s="2" t="n">
+        <v>46017.42774371999</v>
+      </c>
+    </row>
+    <row r="238">
+      <c r="A238" t="inlineStr">
+        <is>
+          <t>sample1.PNG</t>
+        </is>
+      </c>
+      <c r="B238" t="n">
+        <v>1</v>
+      </c>
+      <c r="C238" t="n">
+        <v>73</v>
+      </c>
+      <c r="D238" t="inlineStr">
+        <is>
+          <t>62.95</t>
+        </is>
+      </c>
+      <c r="E238" t="n">
+        <v>0.9923</v>
+      </c>
+      <c r="F238" s="2" t="n">
+        <v>46017.42774371999</v>
+      </c>
+    </row>
+    <row r="239">
+      <c r="A239" t="inlineStr">
+        <is>
+          <t>sample1.PNG</t>
+        </is>
+      </c>
+      <c r="B239" t="n">
+        <v>1</v>
+      </c>
+      <c r="C239" t="n">
+        <v>74</v>
+      </c>
+      <c r="D239" t="inlineStr">
+        <is>
+          <t>62.95</t>
+        </is>
+      </c>
+      <c r="E239" t="n">
+        <v>0.8603</v>
+      </c>
+      <c r="F239" s="2" t="n">
+        <v>46017.42774371999</v>
+      </c>
+    </row>
+    <row r="240">
+      <c r="A240" t="inlineStr">
+        <is>
+          <t>sample1.PNG</t>
+        </is>
+      </c>
+      <c r="B240" t="n">
+        <v>1</v>
+      </c>
+      <c r="C240" t="n">
+        <v>75</v>
+      </c>
+      <c r="D240" t="inlineStr">
+        <is>
+          <t>62415</t>
+        </is>
+      </c>
+      <c r="E240" t="n">
+        <v>0.6682</v>
+      </c>
+      <c r="F240" s="2" t="n">
+        <v>46017.42774371999</v>
+      </c>
+    </row>
+    <row r="241">
+      <c r="A241" t="inlineStr">
+        <is>
+          <t>sample1.PNG</t>
+        </is>
+      </c>
+      <c r="B241" t="n">
+        <v>1</v>
+      </c>
+      <c r="C241" t="n">
+        <v>76</v>
+      </c>
+      <c r="D241" t="inlineStr">
+        <is>
+          <t>62.3</t>
+        </is>
+      </c>
+      <c r="E241" t="n">
+        <v>0.8794</v>
+      </c>
+      <c r="F241" s="2" t="n">
+        <v>46017.42774371999</v>
+      </c>
+    </row>
+    <row r="242">
+      <c r="A242" t="inlineStr">
+        <is>
+          <t>sample1.PNG</t>
+        </is>
+      </c>
+      <c r="B242" t="n">
+        <v>1</v>
+      </c>
+      <c r="C242" t="n">
+        <v>77</v>
+      </c>
+      <c r="D242" t="inlineStr">
+        <is>
+          <t>42,452.660</t>
+        </is>
+      </c>
+      <c r="E242" t="n">
+        <v>0.6391</v>
+      </c>
+      <c r="F242" s="2" t="n">
+        <v>46017.42774371999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>